<commit_message>
Additional companies sent for questionaire
</commit_message>
<xml_diff>
--- a/Alliance Ag & Grain Known Locomotive List.xlsx
+++ b/Alliance Ag & Grain Known Locomotive List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dshi\Documents\GitHub\Web-Scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4FBCA5A-A457-4219-BEE6-F07D3BDE3703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8ACC0F6-7337-41F1-A004-ABDB6A4408DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7AE7A6C5-CD3C-4A7F-8B56-E6AABEC97266}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Leased/Owned</t>
   </si>
@@ -104,12 +104,6 @@
     <t>Company name</t>
   </si>
   <si>
-    <t>Parent company</t>
-  </si>
-  <si>
-    <t>Location County/City</t>
-  </si>
-  <si>
     <t>GMD</t>
   </si>
   <si>
@@ -123,9 +117,6 @@
   </si>
   <si>
     <t>Alliance Ag &amp; Grain Wilroads Elevator</t>
-  </si>
-  <si>
-    <t>Alliance Ag</t>
   </si>
   <si>
     <t>Locomotive ID (Reporting Mark)</t>
@@ -534,137 +525,128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52734771-F49B-4C7A-A606-407A2B80040C}">
-  <dimension ref="A1:Y2"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="A2" sqref="A2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="20" max="24" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="22" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="2" customFormat="1" ht="78" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" s="2" customFormat="1" ht="78" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2">
+        <v>21475</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2">
+        <v>1200</v>
+      </c>
+      <c r="I2" t="s">
         <v>23</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2">
-        <v>21475</v>
-      </c>
-      <c r="I2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2">
-        <v>1200</v>
-      </c>
-      <c r="K2" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q1 L1 I1 J1" xr:uid="{5C3D3E92-F4AC-4A16-8FC4-5885927527EA}">
+    <dataValidation type="whole" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O1 J1 G1 H1" xr:uid="{5C3D3E92-F4AC-4A16-8FC4-5885927527EA}">
       <formula1>2030</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>